<commit_message>
added vid02 partly to my js excel
</commit_message>
<xml_diff>
--- a/jsFundamentals.xlsx
+++ b/jsFundamentals.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="141">
   <si>
     <t>Episode</t>
   </si>
@@ -446,6 +446,42 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>vid-02</t>
+  </si>
+  <si>
+    <t>0.27sec (what happens if you run a js program)</t>
+  </si>
+  <si>
+    <t>we create a js execution context</t>
+  </si>
+  <si>
+    <t>0.53 sec example</t>
+  </si>
+  <si>
+    <t>1.44 (memory execution phase and code execution phase)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>first place if goes through whole program line by line</t>
+  </si>
+  <si>
+    <t>allocates variables and functions a space in memory</t>
+  </si>
+  <si>
+    <t>for variables it is stored as key = variable name and value = undefined</t>
+  </si>
+  <si>
+    <t>for functions it is stored as key = function name and value ={entire function}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.38sec in memory execution phase  </t>
+  </si>
+  <si>
+    <t>5.00sec in code execution phase</t>
   </si>
 </sst>
 </file>
@@ -627,7 +663,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -688,6 +724,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -738,6 +777,44 @@
         <a:xfrm>
           <a:off x="9967628" y="4629150"/>
           <a:ext cx="3024471" cy="2565400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>6349</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9969500" y="10350499"/>
+          <a:ext cx="1460500" cy="1092201"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1036,10 +1113,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1480,7 +1557,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="33" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:9" ht="29" x14ac:dyDescent="0.35">
       <c r="B33" s="20"/>
       <c r="C33" s="15"/>
       <c r="D33" s="15" t="s">
@@ -1490,7 +1567,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:9" ht="58" x14ac:dyDescent="0.35">
       <c r="B34" s="20"/>
       <c r="C34" s="15"/>
       <c r="D34" s="15" t="s">
@@ -1500,7 +1577,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:9" ht="29" x14ac:dyDescent="0.35">
       <c r="B35" s="20"/>
       <c r="C35" s="15"/>
       <c r="D35" s="15" t="s">
@@ -1510,13 +1587,127 @@
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="2:5" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:9" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B36" s="21"/>
       <c r="C36" s="16"/>
       <c r="D36" s="16" t="s">
         <v>126</v>
       </c>
       <c r="E36" s="22"/>
+    </row>
+    <row r="37" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B38" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="E38" s="19"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B39" s="20"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B40" s="20"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="E40" s="14"/>
+    </row>
+    <row r="41" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="B41" s="20"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="E41" s="14"/>
+    </row>
+    <row r="42" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="B42" s="20"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="I42" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="B43" s="20"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="B44" s="20"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="B45" s="20"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="14" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B46" s="20"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="E46" s="14"/>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B47" s="20"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="14"/>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B48" s="20"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="14"/>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B49" s="20"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="14"/>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B50" s="20"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="14"/>
+    </row>
+    <row r="51" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B51" s="21"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>